<commit_message>
guarantee best match same results - concat dataframe match functions
</commit_message>
<xml_diff>
--- a/benchmarking/milk_benchmarking.xlsx
+++ b/benchmarking/milk_benchmarking.xlsx
@@ -182,15 +182,18 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="A:G"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="15.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>